<commit_message>
changes in budget and gdpr
</commit_message>
<xml_diff>
--- a/docs/Week 5/profits.xlsx
+++ b/docs/Week 5/profits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Documents\GitHub\jukevote\docs\Week 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1997218-C1E8-4642-9DD8-116D8D2148B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3637A0D3-4139-4213-855F-67A14801E710}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5768B30F-6220-471E-850D-E341E9DEE88C}"/>
+    <workbookView xWindow="744" yWindow="1476" windowWidth="19836" windowHeight="10356" xr2:uid="{5768B30F-6220-471E-850D-E341E9DEE88C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
                 <c:formatCode>"€"#,##0_);[Red]\("€"#,##0\)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;€&quot;#,##0.00\)">
-                  <c:v>29968</c:v>
+                  <c:v>44968</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19800</c:v>
@@ -833,7 +833,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>13159</c:v>
+                  <c:v>28159</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>39600</c:v>
@@ -1227,7 +1227,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>14023</c:v>
+                  <c:v>29023</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>79200</c:v>
@@ -3447,8 +3447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE31485-FE21-464A-9240-F7E3573AEBF1}">
   <dimension ref="B2:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3490,18 +3490,18 @@
         <v>2000</v>
       </c>
       <c r="E4" s="1">
-        <v>29968</v>
+        <v>44968</v>
       </c>
       <c r="F4" s="2">
         <v>19800</v>
       </c>
       <c r="G4" s="1">
         <f>F4-E4</f>
-        <v>-10168</v>
+        <v>-25168</v>
       </c>
       <c r="H4">
         <f>G4</f>
-        <v>-10168</v>
+        <v>-25168</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -3512,18 +3512,18 @@
         <v>4000</v>
       </c>
       <c r="E5">
-        <v>13159</v>
+        <v>28159</v>
       </c>
       <c r="F5">
         <v>39600</v>
       </c>
       <c r="G5">
         <f>F5-E5</f>
-        <v>26441</v>
+        <v>11441</v>
       </c>
       <c r="H5">
         <f>G5+H4</f>
-        <v>16273</v>
+        <v>-13727</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -3534,18 +3534,18 @@
         <v>8000</v>
       </c>
       <c r="E6">
-        <v>14023</v>
+        <v>29023</v>
       </c>
       <c r="F6">
         <v>79200</v>
       </c>
       <c r="G6">
         <f>F6-E6</f>
-        <v>65177</v>
+        <v>50177</v>
       </c>
       <c r="H6">
         <f>G6+H5</f>
-        <v>81450</v>
+        <v>36450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>